<commit_message>
Report changes: EP test completed
</commit_message>
<xml_diff>
--- a/1-nas/MPI_B_io.xlsx
+++ b/1-nas/MPI_B_io.xlsx
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="14">
   <si>
     <t>dsk/total</t>
   </si>
@@ -77,6 +77,9 @@
   </si>
   <si>
     <t>send</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -1064,11 +1067,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="451964072"/>
-        <c:axId val="451965248"/>
+        <c:axId val="312785744"/>
+        <c:axId val="312764368"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="451964072"/>
+        <c:axId val="312785744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1166,7 +1169,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="451965248"/>
+        <c:crossAx val="312764368"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1174,7 +1177,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="451965248"/>
+        <c:axId val="312764368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1281,7 +1284,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="451964072"/>
+        <c:crossAx val="312785744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:dispUnits>
@@ -1604,11 +1607,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="100"/>
-        <c:axId val="443827920"/>
-        <c:axId val="443828312"/>
+        <c:axId val="313732496"/>
+        <c:axId val="312974712"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="443827920"/>
+        <c:axId val="313732496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1651,7 +1654,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="443828312"/>
+        <c:crossAx val="312974712"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1659,7 +1662,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="443828312"/>
+        <c:axId val="312974712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1710,7 +1713,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="443827920"/>
+        <c:crossAx val="313732496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1836,7 +1839,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2282,11 +2284,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="451975048"/>
-        <c:axId val="451962112"/>
+        <c:axId val="312975496"/>
+        <c:axId val="312975888"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="451975048"/>
+        <c:axId val="312975496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2329,7 +2331,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="451962112"/>
+        <c:crossAx val="312975888"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2337,7 +2339,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="451962112"/>
+        <c:axId val="312975888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2388,7 +2390,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="451975048"/>
+        <c:crossAx val="312975496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2477,7 +2479,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3342,11 +3343,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="451962896"/>
-        <c:axId val="443828704"/>
+        <c:axId val="312976672"/>
+        <c:axId val="312977064"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="451962896"/>
+        <c:axId val="312976672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3388,7 +3389,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="443828704"/>
+        <c:crossAx val="312977064"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3396,7 +3397,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="443828704"/>
+        <c:axId val="312977064"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -3448,7 +3449,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="451962896"/>
+        <c:crossAx val="312976672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3462,7 +3463,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3699,11 +3699,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="428341344"/>
-        <c:axId val="428346440"/>
+        <c:axId val="312977848"/>
+        <c:axId val="312978240"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="428341344"/>
+        <c:axId val="312977848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3746,7 +3746,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="428346440"/>
+        <c:crossAx val="312978240"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3754,7 +3754,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="428346440"/>
+        <c:axId val="312978240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3805,7 +3805,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="428341344"/>
+        <c:crossAx val="312977848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4117,11 +4117,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="455668136"/>
-        <c:axId val="455667744"/>
+        <c:axId val="312979024"/>
+        <c:axId val="312979416"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="455668136"/>
+        <c:axId val="312979024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4164,7 +4164,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="455667744"/>
+        <c:crossAx val="312979416"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4172,7 +4172,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="455667744"/>
+        <c:axId val="312979416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4223,7 +4223,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="455668136"/>
+        <c:crossAx val="312979024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4344,7 +4344,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4526,11 +4525,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="455666960"/>
-        <c:axId val="455666568"/>
+        <c:axId val="312980200"/>
+        <c:axId val="312980592"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="455666960"/>
+        <c:axId val="312980200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4573,7 +4572,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="455666568"/>
+        <c:crossAx val="312980592"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4581,7 +4580,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="455666568"/>
+        <c:axId val="312980592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4632,7 +4631,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="455666960"/>
+        <c:crossAx val="312980200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4721,7 +4720,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5058,11 +5056,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="100"/>
-        <c:axId val="455665784"/>
-        <c:axId val="455665392"/>
+        <c:axId val="312981376"/>
+        <c:axId val="312981768"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="455665784"/>
+        <c:axId val="312981376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5105,7 +5103,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="455665392"/>
+        <c:crossAx val="312981768"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5113,7 +5111,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="455665392"/>
+        <c:axId val="312981768"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -5165,7 +5163,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="455665784"/>
+        <c:crossAx val="312981376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5179,7 +5177,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5431,11 +5428,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="100"/>
-        <c:axId val="455661864"/>
-        <c:axId val="455662256"/>
+        <c:axId val="314457600"/>
+        <c:axId val="314457992"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="455661864"/>
+        <c:axId val="314457600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5478,7 +5475,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="455662256"/>
+        <c:crossAx val="314457992"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5486,7 +5483,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="455662256"/>
+        <c:axId val="314457992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5537,7 +5534,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="455661864"/>
+        <c:crossAx val="314457600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5744,11 +5741,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="421565376"/>
-        <c:axId val="421565768"/>
+        <c:axId val="314458776"/>
+        <c:axId val="314459168"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="421565376"/>
+        <c:axId val="314458776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5791,7 +5788,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="421565768"/>
+        <c:crossAx val="314459168"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5799,7 +5796,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="421565768"/>
+        <c:axId val="314459168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5850,7 +5847,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="421565376"/>
+        <c:crossAx val="314458776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6048,11 +6045,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="455663040"/>
-        <c:axId val="561239312"/>
+        <c:axId val="314459952"/>
+        <c:axId val="314460344"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="455663040"/>
+        <c:axId val="314459952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6095,7 +6092,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="561239312"/>
+        <c:crossAx val="314460344"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6103,7 +6100,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="561239312"/>
+        <c:axId val="314460344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6154,7 +6151,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="455663040"/>
+        <c:crossAx val="314459952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6820,11 +6817,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="477686904"/>
-        <c:axId val="477697096"/>
+        <c:axId val="313252144"/>
+        <c:axId val="313252528"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="477686904"/>
+        <c:axId val="313252144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6922,7 +6919,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="477697096"/>
+        <c:crossAx val="313252528"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6930,7 +6927,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="477697096"/>
+        <c:axId val="313252528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2000000000"/>
@@ -7038,7 +7035,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="477686904"/>
+        <c:crossAx val="313252144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:dispUnits>
@@ -7373,11 +7370,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="561236568"/>
-        <c:axId val="561236960"/>
+        <c:axId val="314461128"/>
+        <c:axId val="314461520"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="561236568"/>
+        <c:axId val="314461128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7420,7 +7417,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="561236960"/>
+        <c:crossAx val="314461520"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7428,7 +7425,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="561236960"/>
+        <c:axId val="314461520"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -7480,7 +7477,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="561236568"/>
+        <c:crossAx val="314461128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7601,7 +7598,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7729,11 +7725,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="561237744"/>
-        <c:axId val="561238136"/>
+        <c:axId val="314462304"/>
+        <c:axId val="314462696"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="561237744"/>
+        <c:axId val="314462304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7776,7 +7772,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="561238136"/>
+        <c:crossAx val="314462696"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7784,7 +7780,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="561238136"/>
+        <c:axId val="314462696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7835,7 +7831,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="561237744"/>
+        <c:crossAx val="314462304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7924,7 +7920,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -8153,11 +8148,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="100"/>
-        <c:axId val="561235784"/>
-        <c:axId val="561236176"/>
+        <c:axId val="314463480"/>
+        <c:axId val="314463872"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="561235784"/>
+        <c:axId val="314463480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8200,7 +8195,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="561236176"/>
+        <c:crossAx val="314463872"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8208,7 +8203,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="561236176"/>
+        <c:axId val="314463872"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -8260,7 +8255,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="561235784"/>
+        <c:crossAx val="314463480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8274,7 +8269,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -8381,7 +8375,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -8514,11 +8507,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="100"/>
-        <c:axId val="457391840"/>
-        <c:axId val="457389880"/>
+        <c:axId val="314464656"/>
+        <c:axId val="314465048"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="457391840"/>
+        <c:axId val="314464656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8561,7 +8554,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="457389880"/>
+        <c:crossAx val="314465048"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8569,7 +8562,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="457389880"/>
+        <c:axId val="314465048"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -8621,7 +8614,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="457391840"/>
+        <c:crossAx val="314464656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8635,7 +8628,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -8742,7 +8734,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -8822,11 +8813,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="329919536"/>
-        <c:axId val="329919928"/>
+        <c:axId val="314699656"/>
+        <c:axId val="314700048"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="329919536"/>
+        <c:axId val="314699656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8869,7 +8860,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="329919928"/>
+        <c:crossAx val="314700048"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8877,7 +8868,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="329919928"/>
+        <c:axId val="314700048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8928,7 +8919,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="329919536"/>
+        <c:crossAx val="314699656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9162,11 +9153,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="457393408"/>
-        <c:axId val="457389488"/>
+        <c:axId val="314700832"/>
+        <c:axId val="314701224"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="457393408"/>
+        <c:axId val="314700832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9209,7 +9200,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="457389488"/>
+        <c:crossAx val="314701224"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9217,7 +9208,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="457389488"/>
+        <c:axId val="314701224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9268,7 +9259,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="457393408"/>
+        <c:crossAx val="314700832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9475,11 +9466,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="442627888"/>
-        <c:axId val="442628280"/>
+        <c:axId val="314702008"/>
+        <c:axId val="314702400"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="442627888"/>
+        <c:axId val="314702008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9522,7 +9513,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="442628280"/>
+        <c:crossAx val="314702400"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9530,7 +9521,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="442628280"/>
+        <c:axId val="314702400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9581,7 +9572,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="442627888"/>
+        <c:crossAx val="314702008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9670,7 +9661,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -9845,11 +9835,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="100"/>
-        <c:axId val="442628672"/>
-        <c:axId val="442629848"/>
+        <c:axId val="314703184"/>
+        <c:axId val="314703576"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="442628672"/>
+        <c:axId val="314703184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9892,7 +9882,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="442629848"/>
+        <c:crossAx val="314703576"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9900,7 +9890,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="442629848"/>
+        <c:axId val="314703576"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -9952,7 +9942,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="442628672"/>
+        <c:crossAx val="314703184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9966,7 +9956,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -10073,7 +10062,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -10174,11 +10162,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="442630632"/>
-        <c:axId val="300208872"/>
+        <c:axId val="314704360"/>
+        <c:axId val="314704752"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="442630632"/>
+        <c:axId val="314704360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10221,7 +10209,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="300208872"/>
+        <c:crossAx val="314704752"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10229,7 +10217,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="300208872"/>
+        <c:axId val="314704752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10280,7 +10268,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="442630632"/>
+        <c:crossAx val="314704360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10441,11 +10429,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="300207304"/>
-        <c:axId val="300208088"/>
+        <c:axId val="314705536"/>
+        <c:axId val="314705928"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="300207304"/>
+        <c:axId val="314705536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10488,7 +10476,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="300208088"/>
+        <c:crossAx val="314705928"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10496,7 +10484,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="300208088"/>
+        <c:axId val="314705928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10547,7 +10535,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="300207304"/>
+        <c:crossAx val="314705536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10944,11 +10932,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="470948040"/>
-        <c:axId val="470946472"/>
+        <c:axId val="313259808"/>
+        <c:axId val="313260192"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="470948040"/>
+        <c:axId val="313259808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11046,7 +11034,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="470946472"/>
+        <c:crossAx val="313260192"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11054,7 +11042,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="470946472"/>
+        <c:axId val="313260192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11161,7 +11149,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="470948040"/>
+        <c:crossAx val="313259808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:dispUnits>
@@ -11436,11 +11424,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="100"/>
-        <c:axId val="425872592"/>
-        <c:axId val="425871808"/>
+        <c:axId val="314706712"/>
+        <c:axId val="315619952"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="425872592"/>
+        <c:axId val="314706712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11483,7 +11471,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="425871808"/>
+        <c:crossAx val="315619952"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11491,7 +11479,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="425871808"/>
+        <c:axId val="315619952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11542,7 +11530,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="425872592"/>
+        <c:crossAx val="314706712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -11790,11 +11778,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="100"/>
-        <c:axId val="459561744"/>
-        <c:axId val="440292104"/>
+        <c:axId val="315620736"/>
+        <c:axId val="315621128"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="459561744"/>
+        <c:axId val="315620736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11837,7 +11825,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="440292104"/>
+        <c:crossAx val="315621128"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11845,7 +11833,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="440292104"/>
+        <c:axId val="315621128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11896,7 +11884,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="459561744"/>
+        <c:crossAx val="315620736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -12094,11 +12082,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="453357160"/>
-        <c:axId val="453356768"/>
+        <c:axId val="315621912"/>
+        <c:axId val="315622304"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="453357160"/>
+        <c:axId val="315621912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12141,7 +12129,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="453356768"/>
+        <c:crossAx val="315622304"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -12149,7 +12137,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="453356768"/>
+        <c:axId val="315622304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12200,7 +12188,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="453357160"/>
+        <c:crossAx val="315621912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -12446,11 +12434,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="100"/>
-        <c:axId val="359657920"/>
-        <c:axId val="469254512"/>
+        <c:axId val="315623088"/>
+        <c:axId val="315623480"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="359657920"/>
+        <c:axId val="315623088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12493,7 +12481,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="469254512"/>
+        <c:crossAx val="315623480"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -12501,7 +12489,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="469254512"/>
+        <c:axId val="315623480"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -12553,7 +12541,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="359657920"/>
+        <c:crossAx val="315623088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -12766,11 +12754,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="329916008"/>
-        <c:axId val="329916792"/>
+        <c:axId val="315624264"/>
+        <c:axId val="315624656"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="329916008"/>
+        <c:axId val="315624264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12813,7 +12801,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="329916792"/>
+        <c:crossAx val="315624656"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -12821,7 +12809,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="329916792"/>
+        <c:axId val="315624656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12872,7 +12860,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="329916008"/>
+        <c:crossAx val="315624264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -13033,11 +13021,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="439426400"/>
-        <c:axId val="361969192"/>
+        <c:axId val="315625440"/>
+        <c:axId val="315625832"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="439426400"/>
+        <c:axId val="315625440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13080,7 +13068,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="361969192"/>
+        <c:crossAx val="315625832"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -13088,7 +13076,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="361969192"/>
+        <c:axId val="315625832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13139,7 +13127,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="439426400"/>
+        <c:crossAx val="315625440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -13349,11 +13337,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="100"/>
-        <c:axId val="361969976"/>
-        <c:axId val="361970368"/>
+        <c:axId val="315626616"/>
+        <c:axId val="315627008"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="361969976"/>
+        <c:axId val="315626616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13396,7 +13384,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="361970368"/>
+        <c:crossAx val="315627008"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -13404,7 +13392,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="361970368"/>
+        <c:axId val="315627008"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -13456,7 +13444,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="361969976"/>
+        <c:crossAx val="315626616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -13582,7 +13570,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -13797,11 +13784,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="361971152"/>
-        <c:axId val="361971544"/>
+        <c:axId val="315751656"/>
+        <c:axId val="315752048"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="361971152"/>
+        <c:axId val="315751656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13844,7 +13831,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="361971544"/>
+        <c:crossAx val="315752048"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -13852,7 +13839,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="361971544"/>
+        <c:axId val="315752048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13903,7 +13890,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="361971152"/>
+        <c:crossAx val="315751656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -13992,7 +13979,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -14395,11 +14381,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="361972328"/>
-        <c:axId val="361972720"/>
+        <c:axId val="315753616"/>
+        <c:axId val="315754008"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="361972328"/>
+        <c:axId val="315753616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14441,7 +14427,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="361972720"/>
+        <c:crossAx val="315754008"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -14449,7 +14435,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="361972720"/>
+        <c:axId val="315754008"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -14501,7 +14487,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="361972328"/>
+        <c:crossAx val="315753616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -14515,7 +14501,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -14780,11 +14765,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="361973504"/>
-        <c:axId val="361973896"/>
+        <c:axId val="315754792"/>
+        <c:axId val="315755184"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="361973504"/>
+        <c:axId val="315754792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14827,7 +14812,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="361973896"/>
+        <c:crossAx val="315755184"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -14835,7 +14820,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="361973896"/>
+        <c:axId val="315755184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14886,7 +14871,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="361973504"/>
+        <c:crossAx val="315754792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -15808,11 +15793,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="561240488"/>
-        <c:axId val="561239704"/>
+        <c:axId val="313725440"/>
+        <c:axId val="313725832"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="561240488"/>
+        <c:axId val="313725440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15910,7 +15895,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="561239704"/>
+        <c:crossAx val="313725832"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -15918,7 +15903,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="561239704"/>
+        <c:axId val="313725832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -16025,7 +16010,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="561240488"/>
+        <c:crossAx val="313725440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:dispUnits>
@@ -16468,11 +16453,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="100"/>
-        <c:axId val="361974680"/>
-        <c:axId val="361975072"/>
+        <c:axId val="315755968"/>
+        <c:axId val="315756360"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="361974680"/>
+        <c:axId val="315755968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -16515,7 +16500,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="361975072"/>
+        <c:crossAx val="315756360"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -16523,7 +16508,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="361975072"/>
+        <c:axId val="315756360"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -16575,7 +16560,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="361974680"/>
+        <c:crossAx val="315755968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -16833,11 +16818,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="361975856"/>
-        <c:axId val="361976248"/>
+        <c:axId val="315757144"/>
+        <c:axId val="315757536"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="361975856"/>
+        <c:axId val="315757144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -16880,7 +16865,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="361976248"/>
+        <c:crossAx val="315757536"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -16888,7 +16873,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="361976248"/>
+        <c:axId val="315757536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -16939,7 +16924,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="361975856"/>
+        <c:crossAx val="315757144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -17275,11 +17260,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="100"/>
-        <c:axId val="329912872"/>
-        <c:axId val="329913264"/>
+        <c:axId val="315758320"/>
+        <c:axId val="315758712"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="329912872"/>
+        <c:axId val="315758320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -17322,7 +17307,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="329913264"/>
+        <c:crossAx val="315758712"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -17330,7 +17315,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="329913264"/>
+        <c:axId val="315758712"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -17382,7 +17367,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="329912872"/>
+        <c:crossAx val="315758320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -17670,11 +17655,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="451977792"/>
-        <c:axId val="470947648"/>
+        <c:axId val="313727792"/>
+        <c:axId val="313727400"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="451977792"/>
+        <c:axId val="313727792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -17717,7 +17702,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="470947648"/>
+        <c:crossAx val="313727400"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -17725,7 +17710,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="470947648"/>
+        <c:axId val="313727400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -17776,7 +17761,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="451977792"/>
+        <c:crossAx val="313727792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -18172,11 +18157,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="100"/>
-        <c:axId val="443824392"/>
-        <c:axId val="443824784"/>
+        <c:axId val="313726616"/>
+        <c:axId val="313728184"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="443824392"/>
+        <c:axId val="313726616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -18219,7 +18204,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="443824784"/>
+        <c:crossAx val="313728184"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -18227,7 +18212,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="443824784"/>
+        <c:axId val="313728184"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -18279,7 +18264,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="443824392"/>
+        <c:crossAx val="313726616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -18400,7 +18385,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -18630,11 +18614,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="443825568"/>
-        <c:axId val="443825960"/>
+        <c:axId val="313728968"/>
+        <c:axId val="313729360"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="443825568"/>
+        <c:axId val="313728968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -18677,7 +18661,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="443825960"/>
+        <c:crossAx val="313729360"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -18685,7 +18669,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="443825960"/>
+        <c:axId val="313729360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -18736,7 +18720,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="443825568"/>
+        <c:crossAx val="313728968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -18825,7 +18809,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -19276,11 +19259,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="100"/>
-        <c:axId val="443826744"/>
-        <c:axId val="443827136"/>
+        <c:axId val="313730144"/>
+        <c:axId val="313730536"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="443826744"/>
+        <c:axId val="313730144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -19323,7 +19306,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="443827136"/>
+        <c:crossAx val="313730536"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -19331,7 +19314,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="443827136"/>
+        <c:axId val="313730536"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -19383,7 +19366,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="443826744"/>
+        <c:crossAx val="313730144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -19397,7 +19380,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -19602,11 +19584,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="451976616"/>
-        <c:axId val="451977008"/>
+        <c:axId val="313731320"/>
+        <c:axId val="313731712"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="451976616"/>
+        <c:axId val="313731320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -19649,7 +19631,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="451977008"/>
+        <c:crossAx val="313731712"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -19657,7 +19639,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="451977008"/>
+        <c:axId val="313731712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -19708,7 +19690,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="451976616"/>
+        <c:crossAx val="313731320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -44547,14 +44529,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="2" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -49740,7 +49728,7 @@
         <v>44090</v>
       </c>
       <c r="N4">
-        <f t="shared" ref="N4:N36" si="0">C4-O4</f>
+        <f t="shared" ref="N4:N31" si="0">C4-O4</f>
         <v>444817408</v>
       </c>
       <c r="O4">
@@ -50972,7 +50960,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="H36" sqref="H36"/>
     </sheetView>
   </sheetViews>
@@ -51064,7 +51052,7 @@
         <v>7426</v>
       </c>
       <c r="L3">
-        <f>C3-M3</f>
+        <f t="shared" ref="L3:L34" si="0">C3-M3</f>
         <v>1052672</v>
       </c>
       <c r="M3">
@@ -51103,7 +51091,7 @@
         <v>0</v>
       </c>
       <c r="L4">
-        <f>C4-M4</f>
+        <f t="shared" si="0"/>
         <v>1048576</v>
       </c>
       <c r="M4">
@@ -51142,7 +51130,7 @@
         <v>0</v>
       </c>
       <c r="L5">
-        <f>C5-M5</f>
+        <f t="shared" si="0"/>
         <v>1060864</v>
       </c>
       <c r="M5">
@@ -51181,7 +51169,7 @@
         <v>0</v>
       </c>
       <c r="L6">
-        <f>C6-M6</f>
+        <f t="shared" si="0"/>
         <v>1060864</v>
       </c>
       <c r="M6">
@@ -51220,7 +51208,7 @@
         <v>0</v>
       </c>
       <c r="L7">
-        <f>C7-M7</f>
+        <f t="shared" si="0"/>
         <v>888832</v>
       </c>
       <c r="M7">
@@ -51259,7 +51247,7 @@
         <v>0</v>
       </c>
       <c r="L8">
-        <f>C8-M8</f>
+        <f t="shared" si="0"/>
         <v>761856</v>
       </c>
       <c r="M8">
@@ -51298,7 +51286,7 @@
         <v>0</v>
       </c>
       <c r="L9">
-        <f>C9-M9</f>
+        <f t="shared" si="0"/>
         <v>626688</v>
       </c>
       <c r="M9">
@@ -51337,7 +51325,7 @@
         <v>0</v>
       </c>
       <c r="L10">
-        <f>C10-M10</f>
+        <f t="shared" si="0"/>
         <v>495616</v>
       </c>
       <c r="M10">
@@ -51376,7 +51364,7 @@
         <v>0</v>
       </c>
       <c r="L11">
-        <f>C11-M11</f>
+        <f t="shared" si="0"/>
         <v>479232</v>
       </c>
       <c r="M11">
@@ -51415,7 +51403,7 @@
         <v>0</v>
       </c>
       <c r="L12">
-        <f>C12-M12</f>
+        <f t="shared" si="0"/>
         <v>479232</v>
       </c>
       <c r="M12">
@@ -51454,7 +51442,7 @@
         <v>0</v>
       </c>
       <c r="L13">
-        <f>C13-M13</f>
+        <f t="shared" si="0"/>
         <v>466944</v>
       </c>
       <c r="M13">
@@ -51493,7 +51481,7 @@
         <v>0</v>
       </c>
       <c r="L14">
-        <f>C14-M14</f>
+        <f t="shared" si="0"/>
         <v>466944</v>
       </c>
       <c r="M14">
@@ -51532,7 +51520,7 @@
         <v>166356</v>
       </c>
       <c r="L15">
-        <f>C15-M15</f>
+        <f t="shared" si="0"/>
         <v>585728</v>
       </c>
       <c r="M15">
@@ -51571,7 +51559,7 @@
         <v>0</v>
       </c>
       <c r="L16">
-        <f>C16-M16</f>
+        <f t="shared" si="0"/>
         <v>585728</v>
       </c>
       <c r="M16">
@@ -51610,7 +51598,7 @@
         <v>252</v>
       </c>
       <c r="L17">
-        <f>C17-M17</f>
+        <f t="shared" si="0"/>
         <v>585728</v>
       </c>
       <c r="M17">
@@ -51649,7 +51637,7 @@
         <v>0</v>
       </c>
       <c r="L18">
-        <f>C18-M18</f>
+        <f t="shared" si="0"/>
         <v>585728</v>
       </c>
       <c r="M18">
@@ -51688,7 +51676,7 @@
         <v>252</v>
       </c>
       <c r="L19">
-        <f>C19-M19</f>
+        <f t="shared" si="0"/>
         <v>573440</v>
       </c>
       <c r="M19">
@@ -51727,7 +51715,7 @@
         <v>0</v>
       </c>
       <c r="L20">
-        <f>C20-M20</f>
+        <f t="shared" si="0"/>
         <v>581632</v>
       </c>
       <c r="M20">
@@ -51766,7 +51754,7 @@
         <v>0</v>
       </c>
       <c r="L21">
-        <f>C21-M21</f>
+        <f t="shared" si="0"/>
         <v>692224</v>
       </c>
       <c r="M21">
@@ -51805,7 +51793,7 @@
         <v>0</v>
       </c>
       <c r="L22">
-        <f>C22-M22</f>
+        <f t="shared" si="0"/>
         <v>692224</v>
       </c>
       <c r="M22">
@@ -51844,7 +51832,7 @@
         <v>0</v>
       </c>
       <c r="L23">
-        <f>C23-M23</f>
+        <f t="shared" si="0"/>
         <v>667648</v>
       </c>
       <c r="M23">
@@ -51883,7 +51871,7 @@
         <v>0</v>
       </c>
       <c r="L24">
-        <f>C24-M24</f>
+        <f t="shared" si="0"/>
         <v>667648</v>
       </c>
       <c r="M24">
@@ -51922,7 +51910,7 @@
         <v>252</v>
       </c>
       <c r="L25">
-        <f>C25-M25</f>
+        <f t="shared" si="0"/>
         <v>659456</v>
       </c>
       <c r="M25">
@@ -51961,7 +51949,7 @@
         <v>0</v>
       </c>
       <c r="L26">
-        <f>C26-M26</f>
+        <f t="shared" si="0"/>
         <v>659456</v>
       </c>
       <c r="M26">
@@ -52000,7 +51988,7 @@
         <v>0</v>
       </c>
       <c r="L27">
-        <f>C27-M27</f>
+        <f t="shared" si="0"/>
         <v>651264</v>
       </c>
       <c r="M27">
@@ -52039,7 +52027,7 @@
         <v>0</v>
       </c>
       <c r="L28">
-        <f>C28-M28</f>
+        <f t="shared" si="0"/>
         <v>651264</v>
       </c>
       <c r="M28">
@@ -52078,7 +52066,7 @@
         <v>0</v>
       </c>
       <c r="L29">
-        <f>C29-M29</f>
+        <f t="shared" si="0"/>
         <v>643072</v>
       </c>
       <c r="M29">
@@ -52117,7 +52105,7 @@
         <v>0</v>
       </c>
       <c r="L30">
-        <f>C30-M30</f>
+        <f t="shared" si="0"/>
         <v>643072</v>
       </c>
       <c r="M30">
@@ -52156,7 +52144,7 @@
         <v>6764</v>
       </c>
       <c r="L31">
-        <f>C31-M31</f>
+        <f t="shared" si="0"/>
         <v>638976</v>
       </c>
       <c r="M31">
@@ -52195,7 +52183,7 @@
         <v>0</v>
       </c>
       <c r="L32">
-        <f>C32-M32</f>
+        <f t="shared" si="0"/>
         <v>634880</v>
       </c>
       <c r="M32">
@@ -52234,7 +52222,7 @@
         <v>0</v>
       </c>
       <c r="L33">
-        <f>C33-M33</f>
+        <f t="shared" si="0"/>
         <v>630784</v>
       </c>
       <c r="M33">
@@ -52273,7 +52261,7 @@
         <v>0</v>
       </c>
       <c r="L34">
-        <f>C34-M34</f>
+        <f t="shared" si="0"/>
         <v>626688</v>
       </c>
       <c r="M34">
@@ -53447,7 +53435,7 @@
         <v>6248</v>
       </c>
       <c r="L3">
-        <f>C3-M3</f>
+        <f t="shared" ref="L3:L34" si="0">C3-M3</f>
         <v>375283712</v>
       </c>
       <c r="M3">
@@ -53486,7 +53474,7 @@
         <v>0</v>
       </c>
       <c r="L4">
-        <f>C4-M4</f>
+        <f t="shared" si="0"/>
         <v>541802496</v>
       </c>
       <c r="M4">
@@ -53525,7 +53513,7 @@
         <v>0</v>
       </c>
       <c r="L5">
-        <f>C5-M5</f>
+        <f t="shared" si="0"/>
         <v>541667328</v>
       </c>
       <c r="M5">
@@ -53564,7 +53552,7 @@
         <v>0</v>
       </c>
       <c r="L6">
-        <f>C6-M6</f>
+        <f t="shared" si="0"/>
         <v>1079554048</v>
       </c>
       <c r="M6">
@@ -53603,7 +53591,7 @@
         <v>406</v>
       </c>
       <c r="L7">
-        <f>C7-M7</f>
+        <f t="shared" si="0"/>
         <v>1348014080</v>
       </c>
       <c r="M7">
@@ -53642,7 +53630,7 @@
         <v>0</v>
       </c>
       <c r="L8">
-        <f>C8-M8</f>
+        <f t="shared" si="0"/>
         <v>1348014080</v>
       </c>
       <c r="M8">
@@ -53681,7 +53669,7 @@
         <v>143242</v>
       </c>
       <c r="L9">
-        <f>C9-M9</f>
+        <f t="shared" si="0"/>
         <v>1348014080</v>
       </c>
       <c r="M9">
@@ -53720,7 +53708,7 @@
         <v>0</v>
       </c>
       <c r="L10">
-        <f>C10-M10</f>
+        <f t="shared" si="0"/>
         <v>1347997696</v>
       </c>
       <c r="M10">
@@ -53759,7 +53747,7 @@
         <v>252</v>
       </c>
       <c r="L11">
-        <f>C11-M11</f>
+        <f t="shared" si="0"/>
         <v>1347870720</v>
       </c>
       <c r="M11">
@@ -53798,7 +53786,7 @@
         <v>0</v>
       </c>
       <c r="L12">
-        <f>C12-M12</f>
+        <f t="shared" si="0"/>
         <v>1347870720</v>
       </c>
       <c r="M12">
@@ -53837,7 +53825,7 @@
         <v>430</v>
       </c>
       <c r="L13">
-        <f>C13-M13</f>
+        <f t="shared" si="0"/>
         <v>1347858432</v>
       </c>
       <c r="M13">
@@ -53876,7 +53864,7 @@
         <v>0</v>
       </c>
       <c r="L14">
-        <f>C14-M14</f>
+        <f t="shared" si="0"/>
         <v>1347858432</v>
       </c>
       <c r="M14">
@@ -53915,7 +53903,7 @@
         <v>0</v>
       </c>
       <c r="L15">
-        <f>C15-M15</f>
+        <f t="shared" si="0"/>
         <v>1347850240</v>
       </c>
       <c r="M15">
@@ -53954,7 +53942,7 @@
         <v>0</v>
       </c>
       <c r="L16">
-        <f>C16-M16</f>
+        <f t="shared" si="0"/>
         <v>1347850240</v>
       </c>
       <c r="M16">
@@ -53993,7 +53981,7 @@
         <v>178</v>
       </c>
       <c r="L17">
-        <f>C17-M17</f>
+        <f t="shared" si="0"/>
         <v>1347710976</v>
       </c>
       <c r="M17">
@@ -54032,7 +54020,7 @@
         <v>0</v>
       </c>
       <c r="L18">
-        <f>C18-M18</f>
+        <f t="shared" si="0"/>
         <v>1347710976</v>
       </c>
       <c r="M18">
@@ -54071,7 +54059,7 @@
         <v>430</v>
       </c>
       <c r="L19">
-        <f>C19-M19</f>
+        <f t="shared" si="0"/>
         <v>1347694592</v>
       </c>
       <c r="M19">
@@ -54110,7 +54098,7 @@
         <v>0</v>
       </c>
       <c r="L20">
-        <f>C20-M20</f>
+        <f t="shared" si="0"/>
         <v>1347694592</v>
       </c>
       <c r="M20">
@@ -54149,7 +54137,7 @@
         <v>178</v>
       </c>
       <c r="L21">
-        <f>C21-M21</f>
+        <f t="shared" si="0"/>
         <v>1347813376</v>
       </c>
       <c r="M21">
@@ -54188,7 +54176,7 @@
         <v>0</v>
       </c>
       <c r="L22">
-        <f>C22-M22</f>
+        <f t="shared" si="0"/>
         <v>1347801088</v>
       </c>
       <c r="M22">
@@ -54227,7 +54215,7 @@
         <v>3948</v>
       </c>
       <c r="L23">
-        <f>C23-M23</f>
+        <f t="shared" si="0"/>
         <v>1347792896</v>
       </c>
       <c r="M23">
@@ -54266,7 +54254,7 @@
         <v>0</v>
       </c>
       <c r="L24">
-        <f>C24-M24</f>
+        <f t="shared" si="0"/>
         <v>1347792896</v>
       </c>
       <c r="M24">
@@ -54305,7 +54293,7 @@
         <v>6024</v>
       </c>
       <c r="L25">
-        <f>C25-M25</f>
+        <f t="shared" si="0"/>
         <v>1347792896</v>
       </c>
       <c r="M25">
@@ -54344,7 +54332,7 @@
         <v>0</v>
       </c>
       <c r="L26">
-        <f>C26-M26</f>
+        <f t="shared" si="0"/>
         <v>1347792896</v>
       </c>
       <c r="M26">
@@ -54383,7 +54371,7 @@
         <v>0</v>
       </c>
       <c r="L27">
-        <f>C27-M27</f>
+        <f t="shared" si="0"/>
         <v>1347776512</v>
       </c>
       <c r="M27">
@@ -54422,7 +54410,7 @@
         <v>0</v>
       </c>
       <c r="L28">
-        <f>C28-M28</f>
+        <f t="shared" si="0"/>
         <v>1347776512</v>
       </c>
       <c r="M28">
@@ -54461,7 +54449,7 @@
         <v>178</v>
       </c>
       <c r="L29">
-        <f>C29-M29</f>
+        <f t="shared" si="0"/>
         <v>1347637248</v>
       </c>
       <c r="M29">
@@ -54500,7 +54488,7 @@
         <v>0</v>
       </c>
       <c r="L30">
-        <f>C30-M30</f>
+        <f t="shared" si="0"/>
         <v>1347637248</v>
       </c>
       <c r="M30">
@@ -54539,7 +54527,7 @@
         <v>430</v>
       </c>
       <c r="L31">
-        <f>C31-M31</f>
+        <f t="shared" si="0"/>
         <v>1347637248</v>
       </c>
       <c r="M31">
@@ -54578,7 +54566,7 @@
         <v>0</v>
       </c>
       <c r="L32">
-        <f>C32-M32</f>
+        <f t="shared" si="0"/>
         <v>1347637248</v>
       </c>
       <c r="M32">
@@ -54617,7 +54605,7 @@
         <v>178</v>
       </c>
       <c r="L33">
-        <f>C33-M33</f>
+        <f t="shared" si="0"/>
         <v>1347629056</v>
       </c>
       <c r="M33">
@@ -54656,7 +54644,7 @@
         <v>0</v>
       </c>
       <c r="L34">
-        <f>C34-M34</f>
+        <f t="shared" si="0"/>
         <v>1347629056</v>
       </c>
       <c r="M34">
@@ -54695,7 +54683,7 @@
         <v>178</v>
       </c>
       <c r="L35">
-        <f>C35-M35</f>
+        <f t="shared" ref="L35:L66" si="1">C35-M35</f>
         <v>1347616768</v>
       </c>
       <c r="M35">
@@ -54734,7 +54722,7 @@
         <v>0</v>
       </c>
       <c r="L36">
-        <f>C36-M36</f>
+        <f t="shared" si="1"/>
         <v>1347616768</v>
       </c>
       <c r="M36">
@@ -54773,7 +54761,7 @@
         <v>178</v>
       </c>
       <c r="L37">
-        <f>C37-M37</f>
+        <f t="shared" si="1"/>
         <v>1347727360</v>
       </c>
       <c r="M37">
@@ -54812,7 +54800,7 @@
         <v>0</v>
       </c>
       <c r="L38">
-        <f>C38-M38</f>
+        <f t="shared" si="1"/>
         <v>1347727360</v>
       </c>
       <c r="M38">
@@ -54851,7 +54839,7 @@
         <v>141338</v>
       </c>
       <c r="L39">
-        <f>C39-M39</f>
+        <f t="shared" si="1"/>
         <v>1347719168</v>
       </c>
       <c r="M39">
@@ -54890,7 +54878,7 @@
         <v>0</v>
       </c>
       <c r="L40">
-        <f>C40-M40</f>
+        <f t="shared" si="1"/>
         <v>1347719168</v>
       </c>
       <c r="M40">
@@ -54929,7 +54917,7 @@
         <v>178</v>
       </c>
       <c r="L41">
-        <f>C41-M41</f>
+        <f t="shared" si="1"/>
         <v>1347842048</v>
       </c>
       <c r="M41">
@@ -54968,7 +54956,7 @@
         <v>0</v>
       </c>
       <c r="L42">
-        <f>C42-M42</f>
+        <f t="shared" si="1"/>
         <v>1347842048</v>
       </c>
       <c r="M42">
@@ -55007,7 +54995,7 @@
         <v>430</v>
       </c>
       <c r="L43">
-        <f>C43-M43</f>
+        <f t="shared" si="1"/>
         <v>1347706880</v>
       </c>
       <c r="M43">
@@ -55046,7 +55034,7 @@
         <v>0</v>
       </c>
       <c r="L44">
-        <f>C44-M44</f>
+        <f t="shared" si="1"/>
         <v>1347706880</v>
       </c>
       <c r="M44">
@@ -55085,7 +55073,7 @@
         <v>178</v>
       </c>
       <c r="L45">
-        <f>C45-M45</f>
+        <f t="shared" si="1"/>
         <v>1347698688</v>
       </c>
       <c r="M45">
@@ -55124,7 +55112,7 @@
         <v>0</v>
       </c>
       <c r="L46">
-        <f>C46-M46</f>
+        <f t="shared" si="1"/>
         <v>1347698688</v>
       </c>
       <c r="M46">
@@ -55163,7 +55151,7 @@
         <v>178</v>
       </c>
       <c r="L47">
-        <f>C47-M47</f>
+        <f t="shared" si="1"/>
         <v>1347674112</v>
       </c>
       <c r="M47">
@@ -55202,7 +55190,7 @@
         <v>0</v>
       </c>
       <c r="L48">
-        <f>C48-M48</f>
+        <f t="shared" si="1"/>
         <v>1347674112</v>
       </c>
       <c r="M48">
@@ -55241,7 +55229,7 @@
         <v>430</v>
       </c>
       <c r="L49">
-        <f>C49-M49</f>
+        <f t="shared" si="1"/>
         <v>1347665920</v>
       </c>
       <c r="M49">
@@ -55280,7 +55268,7 @@
         <v>0</v>
       </c>
       <c r="L50">
-        <f>C50-M50</f>
+        <f t="shared" si="1"/>
         <v>1347661824</v>
       </c>
       <c r="M50">
@@ -55319,7 +55307,7 @@
         <v>448</v>
       </c>
       <c r="L51">
-        <f>C51-M51</f>
+        <f t="shared" si="1"/>
         <v>1347661824</v>
       </c>
       <c r="M51">
@@ -55358,7 +55346,7 @@
         <v>0</v>
       </c>
       <c r="L52">
-        <f>C52-M52</f>
+        <f t="shared" si="1"/>
         <v>1347661824</v>
       </c>
       <c r="M52">
@@ -55397,7 +55385,7 @@
         <v>178</v>
       </c>
       <c r="L53">
-        <f>C53-M53</f>
+        <f t="shared" si="1"/>
         <v>1347641344</v>
       </c>
       <c r="M53">
@@ -55436,7 +55424,7 @@
         <v>0</v>
       </c>
       <c r="L54">
-        <f>C54-M54</f>
+        <f t="shared" si="1"/>
         <v>1347641344</v>
       </c>
       <c r="M54">
@@ -55475,7 +55463,7 @@
         <v>5732</v>
       </c>
       <c r="L55">
-        <f>C55-M55</f>
+        <f t="shared" si="1"/>
         <v>1347641344</v>
       </c>
       <c r="M55">
@@ -55514,7 +55502,7 @@
         <v>0</v>
       </c>
       <c r="L56">
-        <f>C56-M56</f>
+        <f t="shared" si="1"/>
         <v>1347637248</v>
       </c>
       <c r="M56">
@@ -55553,7 +55541,7 @@
         <v>178</v>
       </c>
       <c r="L57">
-        <f>C57-M57</f>
+        <f t="shared" si="1"/>
         <v>1347633152</v>
       </c>
       <c r="M57">
@@ -55592,7 +55580,7 @@
         <v>0</v>
       </c>
       <c r="L58">
-        <f>C58-M58</f>
+        <f t="shared" si="1"/>
         <v>1347633152</v>
       </c>
       <c r="M58">
@@ -55697,7 +55685,7 @@
         <v>0</v>
       </c>
       <c r="L3">
-        <f>C3-M3</f>
+        <f t="shared" ref="L3:L11" si="0">C3-M3</f>
         <v>21446656</v>
       </c>
       <c r="M3">
@@ -55736,7 +55724,7 @@
         <v>3428</v>
       </c>
       <c r="L4">
-        <f>C4-M4</f>
+        <f t="shared" si="0"/>
         <v>50794496</v>
       </c>
       <c r="M4">
@@ -55775,7 +55763,7 @@
         <v>0</v>
       </c>
       <c r="L5">
-        <f>C5-M5</f>
+        <f t="shared" si="0"/>
         <v>80281600</v>
       </c>
       <c r="M5">
@@ -55814,7 +55802,7 @@
         <v>0</v>
       </c>
       <c r="L6">
-        <f>C6-M6</f>
+        <f t="shared" si="0"/>
         <v>111476736</v>
       </c>
       <c r="M6">
@@ -55853,7 +55841,7 @@
         <v>0</v>
       </c>
       <c r="L7">
-        <f>C7-M7</f>
+        <f t="shared" si="0"/>
         <v>269144064</v>
       </c>
       <c r="M7">
@@ -55892,7 +55880,7 @@
         <v>244</v>
       </c>
       <c r="L8">
-        <f>C8-M8</f>
+        <f t="shared" si="0"/>
         <v>277323776</v>
       </c>
       <c r="M8">
@@ -55931,7 +55919,7 @@
         <v>0</v>
       </c>
       <c r="L9">
-        <f>C9-M9</f>
+        <f t="shared" si="0"/>
         <v>277323776</v>
       </c>
       <c r="M9">
@@ -55970,7 +55958,7 @@
         <v>144838</v>
       </c>
       <c r="L10">
-        <f>C10-M10</f>
+        <f t="shared" si="0"/>
         <v>277250048</v>
       </c>
       <c r="M10">
@@ -56009,7 +55997,7 @@
         <v>0</v>
       </c>
       <c r="L11">
-        <f>C11-M11</f>
+        <f t="shared" si="0"/>
         <v>277245952</v>
       </c>
       <c r="M11">
@@ -56114,7 +56102,7 @@
         <v>7582</v>
       </c>
       <c r="L3">
-        <f>C3-$M3</f>
+        <f t="shared" ref="L3:L34" si="0">C3-$M3</f>
         <v>191844352</v>
       </c>
       <c r="M3">
@@ -56153,7 +56141,7 @@
         <v>0</v>
       </c>
       <c r="L4">
-        <f>C4-$M4</f>
+        <f t="shared" si="0"/>
         <v>191844352</v>
       </c>
       <c r="M4">
@@ -56192,7 +56180,7 @@
         <v>0</v>
       </c>
       <c r="L5">
-        <f>C5-$M5</f>
+        <f t="shared" si="0"/>
         <v>191709184</v>
       </c>
       <c r="M5">
@@ -56231,7 +56219,7 @@
         <v>0</v>
       </c>
       <c r="L6">
-        <f>C6-$M6</f>
+        <f t="shared" si="0"/>
         <v>191709184</v>
       </c>
       <c r="M6">
@@ -56270,7 +56258,7 @@
         <v>252</v>
       </c>
       <c r="L7">
-        <f>C7-$M7</f>
+        <f t="shared" si="0"/>
         <v>191688704</v>
       </c>
       <c r="M7">
@@ -56309,7 +56297,7 @@
         <v>0</v>
       </c>
       <c r="L8">
-        <f>C8-$M8</f>
+        <f t="shared" si="0"/>
         <v>191688704</v>
       </c>
       <c r="M8">
@@ -56348,7 +56336,7 @@
         <v>130</v>
       </c>
       <c r="L9">
-        <f>C9-$M9</f>
+        <f t="shared" si="0"/>
         <v>191606784</v>
       </c>
       <c r="M9">
@@ -56387,7 +56375,7 @@
         <v>0</v>
       </c>
       <c r="L10">
-        <f>C10-$M10</f>
+        <f t="shared" si="0"/>
         <v>191614976</v>
       </c>
       <c r="M10">
@@ -56426,7 +56414,7 @@
         <v>12524</v>
       </c>
       <c r="L11">
-        <f>C11-$M11</f>
+        <f t="shared" si="0"/>
         <v>191479808</v>
       </c>
       <c r="M11">
@@ -56465,7 +56453,7 @@
         <v>0</v>
       </c>
       <c r="L12">
-        <f>C12-$M12</f>
+        <f t="shared" si="0"/>
         <v>191479808</v>
       </c>
       <c r="M12">
@@ -56504,7 +56492,7 @@
         <v>4120</v>
       </c>
       <c r="L13">
-        <f>C13-$M13</f>
+        <f t="shared" si="0"/>
         <v>191479808</v>
       </c>
       <c r="M13">
@@ -56543,7 +56531,7 @@
         <v>0</v>
       </c>
       <c r="L14">
-        <f>C14-$M14</f>
+        <f t="shared" si="0"/>
         <v>191479808</v>
       </c>
       <c r="M14">
@@ -56582,7 +56570,7 @@
         <v>130</v>
       </c>
       <c r="L15">
-        <f>C15-$M15</f>
+        <f t="shared" si="0"/>
         <v>191459328</v>
       </c>
       <c r="M15">
@@ -56621,7 +56609,7 @@
         <v>0</v>
       </c>
       <c r="L16">
-        <f>C16-$M16</f>
+        <f t="shared" si="0"/>
         <v>191455232</v>
       </c>
       <c r="M16">
@@ -56660,7 +56648,7 @@
         <v>90</v>
       </c>
       <c r="L17">
-        <f>C17-$M17</f>
+        <f t="shared" si="0"/>
         <v>191320064</v>
       </c>
       <c r="M17">
@@ -56699,7 +56687,7 @@
         <v>0</v>
       </c>
       <c r="L18">
-        <f>C18-$M18</f>
+        <f t="shared" si="0"/>
         <v>191320064</v>
       </c>
       <c r="M18">
@@ -56738,7 +56726,7 @@
         <v>252</v>
       </c>
       <c r="L19">
-        <f>C19-$M19</f>
+        <f t="shared" si="0"/>
         <v>191320064</v>
       </c>
       <c r="M19">
@@ -56777,7 +56765,7 @@
         <v>0</v>
       </c>
       <c r="L20">
-        <f>C20-$M20</f>
+        <f t="shared" si="0"/>
         <v>191320064</v>
       </c>
       <c r="M20">
@@ -56816,7 +56804,7 @@
         <v>0</v>
       </c>
       <c r="L21">
-        <f>C21-$M21</f>
+        <f t="shared" si="0"/>
         <v>191311872</v>
       </c>
       <c r="M21">
@@ -56855,7 +56843,7 @@
         <v>0</v>
       </c>
       <c r="L22">
-        <f>C22-$M22</f>
+        <f t="shared" si="0"/>
         <v>191311872</v>
       </c>
       <c r="M22">
@@ -56894,7 +56882,7 @@
         <v>130</v>
       </c>
       <c r="L23">
-        <f>C23-$M23</f>
+        <f t="shared" si="0"/>
         <v>191168512</v>
       </c>
       <c r="M23">
@@ -56933,7 +56921,7 @@
         <v>0</v>
       </c>
       <c r="L24">
-        <f>C24-$M24</f>
+        <f t="shared" si="0"/>
         <v>191168512</v>
       </c>
       <c r="M24">
@@ -56972,7 +56960,7 @@
         <v>406</v>
       </c>
       <c r="L25">
-        <f>C25-$M25</f>
+        <f t="shared" si="0"/>
         <v>191152128</v>
       </c>
       <c r="M25">
@@ -57011,7 +56999,7 @@
         <v>0</v>
       </c>
       <c r="L26">
-        <f>C26-$M26</f>
+        <f t="shared" si="0"/>
         <v>191152128</v>
       </c>
       <c r="M26">
@@ -57050,7 +57038,7 @@
         <v>142158</v>
       </c>
       <c r="L27">
-        <f>C27-$M27</f>
+        <f t="shared" si="0"/>
         <v>191139840</v>
       </c>
       <c r="M27">
@@ -57089,7 +57077,7 @@
         <v>0</v>
       </c>
       <c r="L28">
-        <f>C28-$M28</f>
+        <f t="shared" si="0"/>
         <v>191139840</v>
       </c>
       <c r="M28">
@@ -57128,7 +57116,7 @@
         <v>130</v>
       </c>
       <c r="L29">
-        <f>C29-$M29</f>
+        <f t="shared" si="0"/>
         <v>191393792</v>
       </c>
       <c r="M29">
@@ -57167,7 +57155,7 @@
         <v>0</v>
       </c>
       <c r="L30">
-        <f>C30-$M30</f>
+        <f t="shared" si="0"/>
         <v>191393792</v>
       </c>
       <c r="M30">
@@ -57206,7 +57194,7 @@
         <v>252</v>
       </c>
       <c r="L31">
-        <f>C31-$M31</f>
+        <f t="shared" si="0"/>
         <v>191385600</v>
       </c>
       <c r="M31">
@@ -57245,7 +57233,7 @@
         <v>0</v>
       </c>
       <c r="L32">
-        <f>C32-$M32</f>
+        <f t="shared" si="0"/>
         <v>191385600</v>
       </c>
       <c r="M32">
@@ -57284,7 +57272,7 @@
         <v>0</v>
       </c>
       <c r="L33">
-        <f>C33-$M33</f>
+        <f t="shared" si="0"/>
         <v>191377408</v>
       </c>
       <c r="M33">
@@ -57323,7 +57311,7 @@
         <v>0</v>
       </c>
       <c r="L34">
-        <f>C34-$M34</f>
+        <f t="shared" si="0"/>
         <v>191373312</v>
       </c>
       <c r="M34">
@@ -57362,7 +57350,7 @@
         <v>130</v>
       </c>
       <c r="L35">
-        <f>C35-$M35</f>
+        <f t="shared" ref="L35:L66" si="1">C35-$M35</f>
         <v>191352832</v>
       </c>
       <c r="M35">
@@ -57401,7 +57389,7 @@
         <v>0</v>
       </c>
       <c r="L36">
-        <f>C36-$M36</f>
+        <f t="shared" si="1"/>
         <v>191348736</v>
       </c>
       <c r="M36">
@@ -57440,7 +57428,7 @@
         <v>252</v>
       </c>
       <c r="L37">
-        <f>C37-$M37</f>
+        <f t="shared" si="1"/>
         <v>191213568</v>
       </c>
       <c r="M37">
@@ -57479,7 +57467,7 @@
         <v>0</v>
       </c>
       <c r="L38">
-        <f>C38-$M38</f>
+        <f t="shared" si="1"/>
         <v>191213568</v>
       </c>
       <c r="M38">
@@ -57518,7 +57506,7 @@
         <v>0</v>
       </c>
       <c r="L39">
-        <f>C39-$M39</f>
+        <f t="shared" si="1"/>
         <v>191213568</v>
       </c>
       <c r="M39">
@@ -57557,7 +57545,7 @@
         <v>0</v>
       </c>
       <c r="L40">
-        <f>C40-$M40</f>
+        <f t="shared" si="1"/>
         <v>191213568</v>
       </c>
       <c r="M40">
@@ -57596,7 +57584,7 @@
         <v>130</v>
       </c>
       <c r="L41">
-        <f>C41-$M41</f>
+        <f t="shared" si="1"/>
         <v>191197184</v>
       </c>
       <c r="M41">
@@ -57635,7 +57623,7 @@
         <v>0</v>
       </c>
       <c r="L42">
-        <f>C42-$M42</f>
+        <f t="shared" si="1"/>
         <v>191197184</v>
       </c>
       <c r="M42">
@@ -57674,7 +57662,7 @@
         <v>7484</v>
       </c>
       <c r="L43">
-        <f>C43-$M43</f>
+        <f t="shared" si="1"/>
         <v>191197184</v>
       </c>
       <c r="M43">
@@ -57713,7 +57701,7 @@
         <v>0</v>
       </c>
       <c r="L44">
-        <f>C44-$M44</f>
+        <f t="shared" si="1"/>
         <v>191197184</v>
       </c>
       <c r="M44">
@@ -57752,7 +57740,7 @@
         <v>0</v>
       </c>
       <c r="L45">
-        <f>C45-$M45</f>
+        <f t="shared" si="1"/>
         <v>191188992</v>
       </c>
       <c r="M45">
@@ -57791,7 +57779,7 @@
         <v>0</v>
       </c>
       <c r="L46">
-        <f>C46-$M46</f>
+        <f t="shared" si="1"/>
         <v>191188992</v>
       </c>
       <c r="M46">
@@ -57830,7 +57818,7 @@
         <v>130</v>
       </c>
       <c r="L47">
-        <f>C47-$M47</f>
+        <f t="shared" si="1"/>
         <v>191172608</v>
       </c>
       <c r="M47">
@@ -57869,7 +57857,7 @@
         <v>0</v>
       </c>
       <c r="L48">
-        <f>C48-$M48</f>
+        <f t="shared" si="1"/>
         <v>191172608</v>
       </c>
       <c r="M48">
@@ -57908,7 +57896,7 @@
         <v>252</v>
       </c>
       <c r="L49">
-        <f>C49-$M49</f>
+        <f t="shared" si="1"/>
         <v>191168512</v>
       </c>
       <c r="M49">
@@ -57947,7 +57935,7 @@
         <v>0</v>
       </c>
       <c r="L50">
-        <f>C50-$M50</f>
+        <f t="shared" si="1"/>
         <v>191168512</v>
       </c>
       <c r="M50">
@@ -57986,7 +57974,7 @@
         <v>240</v>
       </c>
       <c r="L51">
-        <f>C51-$M51</f>
+        <f t="shared" si="1"/>
         <v>191160320</v>
       </c>
       <c r="M51">
@@ -58025,7 +58013,7 @@
         <v>0</v>
       </c>
       <c r="L52">
-        <f>C52-$M52</f>
+        <f t="shared" si="1"/>
         <v>191160320</v>
       </c>
       <c r="M52">
@@ -58064,7 +58052,7 @@
         <v>130</v>
       </c>
       <c r="L53">
-        <f>C53-$M53</f>
+        <f t="shared" si="1"/>
         <v>191152128</v>
       </c>
       <c r="M53">
@@ -58103,7 +58091,7 @@
         <v>0</v>
       </c>
       <c r="L54">
-        <f>C54-$M54</f>
+        <f t="shared" si="1"/>
         <v>191148032</v>
       </c>
       <c r="M54">
@@ -58142,7 +58130,7 @@
         <v>0</v>
       </c>
       <c r="L55">
-        <f>C55-$M55</f>
+        <f t="shared" si="1"/>
         <v>191131648</v>
       </c>
       <c r="M55">
@@ -58181,7 +58169,7 @@
         <v>0</v>
       </c>
       <c r="L56">
-        <f>C56-$M56</f>
+        <f t="shared" si="1"/>
         <v>191131648</v>
       </c>
       <c r="M56">
@@ -58220,7 +58208,7 @@
         <v>140654</v>
       </c>
       <c r="L57">
-        <f>C57-$M57</f>
+        <f t="shared" si="1"/>
         <v>191123456</v>
       </c>
       <c r="M57">
@@ -58259,7 +58247,7 @@
         <v>0</v>
       </c>
       <c r="L58">
-        <f>C58-$M58</f>
+        <f t="shared" si="1"/>
         <v>191123456</v>
       </c>
       <c r="M58">
@@ -58298,7 +58286,7 @@
         <v>382</v>
       </c>
       <c r="L59">
-        <f>C59-$M59</f>
+        <f t="shared" si="1"/>
         <v>191250432</v>
       </c>
       <c r="M59">
@@ -58337,7 +58325,7 @@
         <v>0</v>
       </c>
       <c r="L60">
-        <f>C60-$M60</f>
+        <f t="shared" si="1"/>
         <v>191250432</v>
       </c>
       <c r="M60">
@@ -58376,7 +58364,7 @@
         <v>252</v>
       </c>
       <c r="L61">
-        <f>C61-$M61</f>
+        <f t="shared" si="1"/>
         <v>191238144</v>
       </c>
       <c r="M61">
@@ -58415,7 +58403,7 @@
         <v>0</v>
       </c>
       <c r="L62">
-        <f>C62-$M62</f>
+        <f t="shared" si="1"/>
         <v>191238144</v>
       </c>
       <c r="M62">
@@ -58454,7 +58442,7 @@
         <v>0</v>
       </c>
       <c r="L63">
-        <f>C63-$M63</f>
+        <f t="shared" si="1"/>
         <v>191229952</v>
       </c>
       <c r="M63">
@@ -58493,7 +58481,7 @@
         <v>0</v>
       </c>
       <c r="L64">
-        <f>C64-$M64</f>
+        <f t="shared" si="1"/>
         <v>191229952</v>
       </c>
       <c r="M64">
@@ -58532,7 +58520,7 @@
         <v>130</v>
       </c>
       <c r="L65">
-        <f>C65-$M65</f>
+        <f t="shared" si="1"/>
         <v>191221760</v>
       </c>
       <c r="M65">
@@ -58571,7 +58559,7 @@
         <v>0</v>
       </c>
       <c r="L66">
-        <f>C66-$M66</f>
+        <f t="shared" si="1"/>
         <v>191221760</v>
       </c>
       <c r="M66">
@@ -58610,7 +58598,7 @@
         <v>252</v>
       </c>
       <c r="L67">
-        <f>C67-$M67</f>
+        <f t="shared" ref="L67:L98" si="2">C67-$M67</f>
         <v>191205376</v>
       </c>
       <c r="M67">
@@ -58649,7 +58637,7 @@
         <v>0</v>
       </c>
       <c r="L68">
-        <f>C68-$M68</f>
+        <f t="shared" si="2"/>
         <v>191205376</v>
       </c>
       <c r="M68">
@@ -58688,7 +58676,7 @@
         <v>406</v>
       </c>
       <c r="L69">
-        <f>C69-$M69</f>
+        <f t="shared" si="2"/>
         <v>191197184</v>
       </c>
       <c r="M69">
@@ -58727,7 +58715,7 @@
         <v>0</v>
       </c>
       <c r="L70">
-        <f>C70-$M70</f>
+        <f t="shared" si="2"/>
         <v>191205376</v>
       </c>
       <c r="M70">
@@ -58766,7 +58754,7 @@
         <v>3770</v>
       </c>
       <c r="L71">
-        <f>C71-$M71</f>
+        <f t="shared" si="2"/>
         <v>191197184</v>
       </c>
       <c r="M71">
@@ -58805,7 +58793,7 @@
         <v>0</v>
       </c>
       <c r="L72">
-        <f>C72-$M72</f>
+        <f t="shared" si="2"/>
         <v>191205376</v>
       </c>
       <c r="M72">
@@ -58844,7 +58832,7 @@
         <v>6968</v>
       </c>
       <c r="L73">
-        <f>C73-$M73</f>
+        <f t="shared" si="2"/>
         <v>191193088</v>
       </c>
       <c r="M73">
@@ -58883,7 +58871,7 @@
         <v>0</v>
       </c>
       <c r="L74">
-        <f>C74-$M74</f>
+        <f t="shared" si="2"/>
         <v>191193088</v>
       </c>
       <c r="M74">
@@ -58922,7 +58910,7 @@
         <v>0</v>
       </c>
       <c r="L75">
-        <f>C75-$M75</f>
+        <f t="shared" si="2"/>
         <v>191176704</v>
       </c>
       <c r="M75">
@@ -58961,7 +58949,7 @@
         <v>0</v>
       </c>
       <c r="L76">
-        <f>C76-$M76</f>
+        <f t="shared" si="2"/>
         <v>191176704</v>
       </c>
       <c r="M76">
@@ -59000,7 +58988,7 @@
         <v>0</v>
       </c>
       <c r="L77">
-        <f>C77-$M77</f>
+        <f t="shared" si="2"/>
         <v>191168512</v>
       </c>
       <c r="M77">
@@ -59039,7 +59027,7 @@
         <v>0</v>
       </c>
       <c r="L78">
-        <f>C78-$M78</f>
+        <f t="shared" si="2"/>
         <v>191168512</v>
       </c>
       <c r="M78">
@@ -59078,7 +59066,7 @@
         <v>382</v>
       </c>
       <c r="L79">
-        <f>C79-$M79</f>
+        <f t="shared" si="2"/>
         <v>191168512</v>
       </c>
       <c r="M79">
@@ -59117,7 +59105,7 @@
         <v>0</v>
       </c>
       <c r="L80">
-        <f>C80-$M80</f>
+        <f t="shared" si="2"/>
         <v>191168512</v>
       </c>
       <c r="M80">
@@ -59156,7 +59144,7 @@
         <v>0</v>
       </c>
       <c r="L81">
-        <f>C81-$M81</f>
+        <f t="shared" si="2"/>
         <v>191160320</v>
       </c>
       <c r="M81">
@@ -59195,7 +59183,7 @@
         <v>0</v>
       </c>
       <c r="L82">
-        <f>C82-$M82</f>
+        <f t="shared" si="2"/>
         <v>191160320</v>
       </c>
       <c r="M82">
@@ -59234,7 +59222,7 @@
         <v>0</v>
       </c>
       <c r="L83">
-        <f>C83-$M83</f>
+        <f t="shared" si="2"/>
         <v>191152128</v>
       </c>
       <c r="M83">
@@ -59273,7 +59261,7 @@
         <v>0</v>
       </c>
       <c r="L84">
-        <f>C84-$M84</f>
+        <f t="shared" si="2"/>
         <v>191152128</v>
       </c>
       <c r="M84">
@@ -59312,7 +59300,7 @@
         <v>130</v>
       </c>
       <c r="L85">
-        <f>C85-$M85</f>
+        <f t="shared" si="2"/>
         <v>191131648</v>
       </c>
       <c r="M85">
@@ -59351,7 +59339,7 @@
         <v>0</v>
       </c>
       <c r="L86">
-        <f>C86-$M86</f>
+        <f t="shared" si="2"/>
         <v>191131648</v>
       </c>
       <c r="M86">
@@ -59390,7 +59378,7 @@
         <v>143250</v>
       </c>
       <c r="L87">
-        <f>C87-$M87</f>
+        <f t="shared" si="2"/>
         <v>191250432</v>
       </c>
       <c r="M87">
@@ -59429,7 +59417,7 @@
         <v>0</v>
       </c>
       <c r="L88">
-        <f>C88-$M88</f>
+        <f t="shared" si="2"/>
         <v>191250432</v>
       </c>
       <c r="M88">
@@ -59468,7 +59456,7 @@
         <v>252</v>
       </c>
       <c r="L89">
-        <f>C89-$M89</f>
+        <f t="shared" si="2"/>
         <v>191250432</v>
       </c>
       <c r="M89">
@@ -59507,7 +59495,7 @@
         <v>0</v>
       </c>
       <c r="L90">
-        <f>C90-$M90</f>
+        <f t="shared" si="2"/>
         <v>191250432</v>
       </c>
       <c r="M90">
@@ -59546,7 +59534,7 @@
         <v>382</v>
       </c>
       <c r="L91">
-        <f>C91-$M91</f>
+        <f t="shared" si="2"/>
         <v>191242240</v>
       </c>
       <c r="M91">
@@ -59585,7 +59573,7 @@
         <v>0</v>
       </c>
       <c r="L92">
-        <f>C92-$M92</f>
+        <f t="shared" si="2"/>
         <v>191238144</v>
       </c>
       <c r="M92">
@@ -59624,7 +59612,7 @@
         <v>0</v>
       </c>
       <c r="L93">
-        <f>C93-$M93</f>
+        <f t="shared" si="2"/>
         <v>191229952</v>
       </c>
       <c r="M93">
@@ -59663,7 +59651,7 @@
         <v>0</v>
       </c>
       <c r="L94">
-        <f>C94-$M94</f>
+        <f t="shared" si="2"/>
         <v>191229952</v>
       </c>
       <c r="M94">
@@ -59702,7 +59690,7 @@
         <v>42</v>
       </c>
       <c r="L95">
-        <f>C95-$M95</f>
+        <f t="shared" si="2"/>
         <v>191201280</v>
       </c>
       <c r="M95">
@@ -59741,7 +59729,7 @@
         <v>0</v>
       </c>
       <c r="L96">
-        <f>C96-$M96</f>
+        <f t="shared" si="2"/>
         <v>191201280</v>
       </c>
       <c r="M96">
@@ -59780,7 +59768,7 @@
         <v>382</v>
       </c>
       <c r="L97">
-        <f>C97-$M97</f>
+        <f t="shared" si="2"/>
         <v>191184896</v>
       </c>
       <c r="M97">
@@ -59819,7 +59807,7 @@
         <v>0</v>
       </c>
       <c r="L98">
-        <f>C98-$M98</f>
+        <f t="shared" si="2"/>
         <v>191184896</v>
       </c>
       <c r="M98">
@@ -59858,7 +59846,7 @@
         <v>0</v>
       </c>
       <c r="L99">
-        <f>C99-$M99</f>
+        <f t="shared" ref="L99:L127" si="3">C99-$M99</f>
         <v>191184896</v>
       </c>
       <c r="M99">
@@ -59897,7 +59885,7 @@
         <v>0</v>
       </c>
       <c r="L100">
-        <f>C100-$M100</f>
+        <f t="shared" si="3"/>
         <v>191184896</v>
       </c>
       <c r="M100">
@@ -59936,7 +59924,7 @@
         <v>0</v>
       </c>
       <c r="L101">
-        <f>C101-$M101</f>
+        <f t="shared" si="3"/>
         <v>191176704</v>
       </c>
       <c r="M101">
@@ -59975,7 +59963,7 @@
         <v>0</v>
       </c>
       <c r="L102">
-        <f>C102-$M102</f>
+        <f t="shared" si="3"/>
         <v>191184896</v>
       </c>
       <c r="M102">
@@ -60014,7 +60002,7 @@
         <v>6088</v>
       </c>
       <c r="L103">
-        <f>C103-$M103</f>
+        <f t="shared" si="3"/>
         <v>191176704</v>
       </c>
       <c r="M103">
@@ -60053,7 +60041,7 @@
         <v>0</v>
       </c>
       <c r="L104">
-        <f>C104-$M104</f>
+        <f t="shared" si="3"/>
         <v>191176704</v>
       </c>
       <c r="M104">
@@ -60092,7 +60080,7 @@
         <v>0</v>
       </c>
       <c r="L105">
-        <f>C105-$M105</f>
+        <f t="shared" si="3"/>
         <v>191168512</v>
       </c>
       <c r="M105">
@@ -60131,7 +60119,7 @@
         <v>0</v>
       </c>
       <c r="L106">
-        <f>C106-$M106</f>
+        <f t="shared" si="3"/>
         <v>191168512</v>
       </c>
       <c r="M106">
@@ -60170,7 +60158,7 @@
         <v>0</v>
       </c>
       <c r="L107">
-        <f>C107-$M107</f>
+        <f t="shared" si="3"/>
         <v>191148032</v>
       </c>
       <c r="M107">
@@ -60209,7 +60197,7 @@
         <v>0</v>
       </c>
       <c r="L108">
-        <f>C108-$M108</f>
+        <f t="shared" si="3"/>
         <v>191148032</v>
       </c>
       <c r="M108">
@@ -60248,7 +60236,7 @@
         <v>382</v>
       </c>
       <c r="L109">
-        <f>C109-$M109</f>
+        <f t="shared" si="3"/>
         <v>191148032</v>
       </c>
       <c r="M109">
@@ -60287,7 +60275,7 @@
         <v>0</v>
       </c>
       <c r="L110">
-        <f>C110-$M110</f>
+        <f t="shared" si="3"/>
         <v>191143936</v>
       </c>
       <c r="M110">
@@ -60326,7 +60314,7 @@
         <v>240</v>
       </c>
       <c r="L111">
-        <f>C111-$M111</f>
+        <f t="shared" si="3"/>
         <v>191139840</v>
       </c>
       <c r="M111">
@@ -60365,7 +60353,7 @@
         <v>0</v>
       </c>
       <c r="L112">
-        <f>C112-$M112</f>
+        <f t="shared" si="3"/>
         <v>191139840</v>
       </c>
       <c r="M112">
@@ -60404,7 +60392,7 @@
         <v>0</v>
       </c>
       <c r="L113">
-        <f>C113-$M113</f>
+        <f t="shared" si="3"/>
         <v>191123456</v>
       </c>
       <c r="M113">
@@ -60443,7 +60431,7 @@
         <v>0</v>
       </c>
       <c r="L114">
-        <f>C114-$M114</f>
+        <f t="shared" si="3"/>
         <v>191119360</v>
       </c>
       <c r="M114">
@@ -60482,7 +60470,7 @@
         <v>536</v>
       </c>
       <c r="L115">
-        <f>C115-$M115</f>
+        <f t="shared" si="3"/>
         <v>191107072</v>
       </c>
       <c r="M115">
@@ -60521,7 +60509,7 @@
         <v>0</v>
       </c>
       <c r="L116">
-        <f>C116-$M116</f>
+        <f t="shared" si="3"/>
         <v>191107072</v>
       </c>
       <c r="M116">
@@ -60560,7 +60548,7 @@
         <v>141540</v>
       </c>
       <c r="L117">
-        <f>C117-$M117</f>
+        <f t="shared" si="3"/>
         <v>191107072</v>
       </c>
       <c r="M117">
@@ -60599,7 +60587,7 @@
         <v>0</v>
       </c>
       <c r="L118">
-        <f>C118-$M118</f>
+        <f t="shared" si="3"/>
         <v>191107072</v>
       </c>
       <c r="M118">
@@ -60638,7 +60626,7 @@
         <v>252</v>
       </c>
       <c r="L119">
-        <f>C119-$M119</f>
+        <f t="shared" si="3"/>
         <v>191102976</v>
       </c>
       <c r="M119">
@@ -60677,7 +60665,7 @@
         <v>0</v>
       </c>
       <c r="L120">
-        <f>C120-$M120</f>
+        <f t="shared" si="3"/>
         <v>191102976</v>
       </c>
       <c r="M120">
@@ -60716,7 +60704,7 @@
         <v>382</v>
       </c>
       <c r="L121">
-        <f>C121-$M121</f>
+        <f t="shared" si="3"/>
         <v>191221760</v>
       </c>
       <c r="M121">
@@ -60755,7 +60743,7 @@
         <v>0</v>
       </c>
       <c r="L122">
-        <f>C122-$M122</f>
+        <f t="shared" si="3"/>
         <v>191221760</v>
       </c>
       <c r="M122">
@@ -60794,7 +60782,7 @@
         <v>0</v>
       </c>
       <c r="L123">
-        <f>C123-$M123</f>
+        <f t="shared" si="3"/>
         <v>191213568</v>
       </c>
       <c r="M123">
@@ -60833,7 +60821,7 @@
         <v>0</v>
       </c>
       <c r="L124">
-        <f>C124-$M124</f>
+        <f t="shared" si="3"/>
         <v>191213568</v>
       </c>
       <c r="M124">
@@ -60872,7 +60860,7 @@
         <v>0</v>
       </c>
       <c r="L125">
-        <f>C125-$M125</f>
+        <f t="shared" si="3"/>
         <v>191205376</v>
       </c>
       <c r="M125">
@@ -60911,7 +60899,7 @@
         <v>0</v>
       </c>
       <c r="L126">
-        <f>C126-$M126</f>
+        <f t="shared" si="3"/>
         <v>191205376</v>
       </c>
       <c r="M126">
@@ -60950,7 +60938,7 @@
         <v>252</v>
       </c>
       <c r="L127">
-        <f>C127-$M127</f>
+        <f t="shared" si="3"/>
         <v>191062016</v>
       </c>
       <c r="M127">

</xml_diff>